<commit_message>
Actualización de libro de Excel
Add caso extraordinario 4 y caso error 4
</commit_message>
<xml_diff>
--- a/Liquidador-de-Nómina.xlsx
+++ b/Liquidador-de-Nómina.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/A0A66C4E88FB0D17/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="8_{FDE5CBCE-8AF8-41F9-BF5D-FC43121CB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B44892F6-E375-4FA8-AF39-0AC77E441CD6}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{FDE5CBCE-8AF8-41F9-BF5D-FC43121CB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B35B6DDB-FF38-4818-AFFB-1634E97145A2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{ACC24777-1EF7-4777-BC9E-05463E1B662D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC24777-1EF7-4777-BC9E-05463E1B662D}"/>
   </bookViews>
   <sheets>
     <sheet name="Nómina" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>Luis Guerra</author>
   </authors>
   <commentList>
-    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{3F73A23E-1A38-42FF-97E5-032C577012CD}">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{3F73A23E-1A38-42FF-97E5-032C577012CD}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{D2D42BE4-7AE4-4D9C-9875-CE9708F44863}">
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{D2D42BE4-7AE4-4D9C-9875-CE9708F44863}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{0D6D5E46-2C5C-4CFB-BE45-37646A23583C}">
+    <comment ref="S6" authorId="0" shapeId="0" xr:uid="{0D6D5E46-2C5C-4CFB-BE45-37646A23583C}">
       <text>
         <r>
           <rPr>
@@ -168,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{0FCDE7A4-F2D6-4E7A-9FC5-0142DE5B9292}">
+    <comment ref="K15" authorId="0" shapeId="0" xr:uid="{0FCDE7A4-F2D6-4E7A-9FC5-0142DE5B9292}">
       <text>
         <r>
           <rPr>
@@ -189,6 +189,54 @@
           </rPr>
           <t xml:space="preserve">
 Préstamo con 60 cuotas (plazo extenso).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N16" authorId="0" shapeId="0" xr:uid="{68F7CC55-DE81-4AE1-B2D5-3EA8044784A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Guerra:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Si el trabajor tiene horas extras en diferentes turnos estas se suman y se aplica el factor correspondiente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{7ABD7D10-FBD1-4784-8422-DD847EE745D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luis Guerra:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El limite al mes es de 30 horas y el empleado tiene 32</t>
         </r>
       </text>
     </comment>
@@ -215,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>Entradas</t>
   </si>
@@ -380,6 +428,15 @@
   </si>
   <si>
     <t>Tasa de interes (Anual)</t>
+  </si>
+  <si>
+    <t>Horas extras adiccionales</t>
+  </si>
+  <si>
+    <t>Tipo de hora extra adiccional</t>
+  </si>
+  <si>
+    <t>#ERROR: Límite Legal de Horas Extras Excedido</t>
   </si>
 </sst>
 </file>
@@ -390,7 +447,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;XDR&quot;* #,##0.00_-;\-&quot;XDR&quot;* #,##0.00_-;_-&quot;XDR&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +497,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -617,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -692,9 +762,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -744,8 +811,8 @@
     <xf numFmtId="9" fontId="4" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -774,9 +841,22 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1132,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10311B7A-29B6-449E-A833-BFA5BF788BF0}">
-  <dimension ref="B4:S25"/>
+  <dimension ref="B4:U26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,65 +1224,70 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="6" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="49" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-    </row>
-    <row r="6" spans="2:18" ht="27" x14ac:dyDescent="0.25">
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+    </row>
+    <row r="6" spans="2:20" ht="27" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1219,44 +1304,50 @@
         <v>26</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="57" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1271,60 +1362,62 @@
       <c r="F7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="55"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="10">
         <f>IF(C7="Empleado nuevo",50000,IF(C7="Empleado antiguo",100000,IF(C7="Administrador",150000,0)))</f>
         <v>50000</v>
       </c>
-      <c r="H7" s="8">
+      <c r="J7" s="8">
         <v>500000</v>
       </c>
-      <c r="I7" s="14">
+      <c r="K7" s="14">
         <v>12</v>
       </c>
-      <c r="J7" s="6">
+      <c r="L7" s="6">
         <v>0.06</v>
       </c>
-      <c r="K7" s="42">
-        <f>D7+M7+L7-N7-O7-P7</f>
+      <c r="M7" s="41">
+        <f>D7+O7+N7-P7-Q7-R7</f>
         <v>1741902.5083333333</v>
       </c>
-      <c r="L7" s="9">
-        <f>E7*(D7/240)*IF(F7="Diurnas",1.25,IF(F7="Nocturnas",1.75,IF(F7="Festivas",2.5,0)))</f>
+      <c r="N7" s="9">
+        <f>(E7*(D7/240)*IF(F7="Diurnas",1.25,IF(F7="Nocturnas",1.75,IF(F7="Festivas",2.5,0)))) + IF(G7 &gt; 0,G7*(D7/240)*IF(H7="Diurnas",1.25,IF(H7="Nocturnas",1.75,IF(H7="Festivas",2.5,0))),0)</f>
         <v>42968.75</v>
       </c>
-      <c r="M7" s="8">
-        <f>IF(D7 &lt;= (Adiccionales!$J$6*2),(G7+Adiccionales!$H$6),G7)</f>
+      <c r="O7" s="8">
+        <f>IF(D7 &lt;= (Adiccionales!$J$6*2),(I7+Adiccionales!$H$6),I7)</f>
         <v>250000</v>
       </c>
-      <c r="N7" s="10">
-        <f>IF(I7=0,H7,(H7*(1+J7)/I7))</f>
+      <c r="P7" s="10">
+        <f>IF(K7=0,J7,(J7*(1+L7)/K7))</f>
         <v>44166.666666666664</v>
       </c>
-      <c r="O7" s="8">
+      <c r="Q7" s="8">
         <f>(D7*Adiccionales!$F$6) + (D7*Adiccionales!$G$6)</f>
         <v>132000</v>
       </c>
-      <c r="P7" s="10">
-        <f>IF(Q7 &lt;= Adiccionales!$G$11,
+      <c r="R7" s="10">
+        <f>IF(S7 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q7 &lt;= Adiccionales!$H$11,
-       (Q7 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q7 - Adiccionales!$H$11) * 0.02)
+    IF(S7 &lt;= Adiccionales!$H$11,
+       (S7 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S7 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>24899.575000000001</v>
       </c>
-      <c r="Q7" s="8">
-        <f>D7+G7+L7</f>
+      <c r="S7" s="8">
+        <f>D7+I7+N7</f>
         <v>1742968.75</v>
       </c>
-      <c r="R7" s="10" t="str">
+      <c r="T7" s="10" t="str">
         <f>ROUND(D7/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>33.13 UVT</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="57" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1337,60 +1430,62 @@
         <v>0</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="10">
-        <f t="shared" ref="G8:G22" si="0">IF(C8="Empleado nuevo",50000,IF(C8="Empleado antiguo",100000,IF(C8="Administrador",150000,0)))</f>
+      <c r="G8" s="55"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="10">
+        <f t="shared" ref="I8:I22" si="0">IF(C8="Empleado nuevo",50000,IF(C8="Empleado antiguo",100000,IF(C8="Administrador",150000,0)))</f>
         <v>50000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="J8" s="8">
         <v>600000</v>
       </c>
-      <c r="I8" s="14">
+      <c r="K8" s="14">
         <v>12</v>
       </c>
-      <c r="J8" s="6">
+      <c r="L8" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K8" s="42">
-        <f>D8+M8+L8-N8-O8-P8</f>
+      <c r="M8" s="41">
+        <f>D8+O8+N8-P8-Q8-R8</f>
         <v>1780459.8</v>
       </c>
-      <c r="L8" s="9">
-        <f>E8*(D8/240)*IF(F8="Diurnas",1.25,IF(F8="Nocturnas",1.75,IF(F8="Festivas",2.5,0)))</f>
+      <c r="N8" s="9">
+        <f t="shared" ref="N8:N22" si="1">(E8*(D8/240)*IF(F8="Diurnas",1.25,IF(F8="Nocturnas",1.75,IF(F8="Festivas",2.5,0)))) + IF(G8 &gt; 0,G8*(D8/240)*IF(H8="Diurnas",1.25,IF(H8="Nocturnas",1.75,IF(H8="Festivas",2.5,0))),0)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="8">
-        <f>IF(D8 &lt;= (Adiccionales!$J$6*2),(G8+Adiccionales!$H$6),G8)</f>
+      <c r="O8" s="8">
+        <f>IF(D8 &lt;= (Adiccionales!$J$6*2),(I8+Adiccionales!$H$6),I8)</f>
         <v>250000</v>
       </c>
-      <c r="N8" s="10">
-        <f t="shared" ref="N8:N22" si="1">IF(I8=0,H8,(H8*(1+J8)/I8))</f>
+      <c r="P8" s="10">
+        <f t="shared" ref="P8:P22" si="2">IF(K8=0,J8,(J8*(1+L8)/K8))</f>
         <v>53500</v>
       </c>
-      <c r="O8" s="8">
+      <c r="Q8" s="8">
         <f>(D8*Adiccionales!$F$6) + (D8*Adiccionales!$G$6)</f>
         <v>140000</v>
       </c>
-      <c r="P8" s="10">
-        <f>IF(Q8 &lt;= Adiccionales!$G$11,
+      <c r="R8" s="10">
+        <f>IF(S8 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q8 &lt;= Adiccionales!$H$11,
-       (Q8 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q8 - Adiccionales!$H$11) * 0.02)
+    IF(S8 &lt;= Adiccionales!$H$11,
+       (S8 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S8 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>26040.2</v>
       </c>
-      <c r="Q8" s="8">
-        <f t="shared" ref="Q8:Q22" si="2">D8+G8+L8</f>
+      <c r="S8" s="8">
+        <f t="shared" ref="S8:S22" si="3">D8+I8+N8</f>
         <v>1800000</v>
       </c>
-      <c r="R8" s="10" t="str">
+      <c r="T8" s="10" t="str">
         <f>ROUND(D8/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>35.14 UVT</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="57" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1405,60 +1500,62 @@
       <c r="F9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="55"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="H9" s="8">
+      <c r="J9" s="8">
         <v>100000</v>
       </c>
-      <c r="I9" s="14">
+      <c r="K9" s="14">
         <v>12</v>
       </c>
-      <c r="J9" s="6">
+      <c r="L9" s="6">
         <v>0.06</v>
       </c>
-      <c r="K9" s="42">
-        <f>D9+M9+L9-N9-O9-P9</f>
+      <c r="M9" s="41">
+        <f>D9+O9+N9-P9-Q9-R9</f>
         <v>4360626.4666666668</v>
       </c>
-      <c r="L9" s="9">
-        <f>E9*(D9/240)*IF(F9="Diurnas",1.25,IF(F9="Nocturnas",1.75,IF(F9="Festivas",2.5,0)))</f>
+      <c r="N9" s="9">
+        <f t="shared" si="1"/>
         <v>625000.00000000012</v>
       </c>
-      <c r="M9" s="8">
-        <f>IF(D9 &lt;= (Adiccionales!$J$6*2),(G9+Adiccionales!$H$6),G9)</f>
+      <c r="O9" s="8">
+        <f>IF(D9 &lt;= (Adiccionales!$J$6*2),(I9+Adiccionales!$H$6),I9)</f>
         <v>150000</v>
       </c>
-      <c r="N9" s="10">
-        <f t="shared" si="1"/>
+      <c r="P9" s="10">
+        <f t="shared" si="2"/>
         <v>8833.3333333333339</v>
       </c>
-      <c r="O9" s="8">
+      <c r="Q9" s="8">
         <f>(D9*Adiccionales!$F$6) + (D9*Adiccionales!$G$6)</f>
         <v>320000</v>
       </c>
-      <c r="P9" s="10">
-        <f>IF(Q9 &lt;= Adiccionales!$G$11,
+      <c r="R9" s="10">
+        <f>IF(S9 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q9 &lt;= Adiccionales!$H$11,
-       (Q9 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q9 - Adiccionales!$H$11) * 0.02)
+    IF(S9 &lt;= Adiccionales!$H$11,
+       (S9 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S9 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>85540.200000000012</v>
       </c>
-      <c r="Q9" s="8">
-        <f t="shared" si="2"/>
+      <c r="S9" s="8">
+        <f t="shared" si="3"/>
         <v>4775000</v>
       </c>
-      <c r="R9" s="10" t="str">
+      <c r="T9" s="10" t="str">
         <f>ROUND(D9/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>80.32 UVT</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1473,100 +1570,106 @@
       <c r="F10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="55"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="10">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="H10" s="8">
+      <c r="J10" s="8">
         <v>0</v>
       </c>
-      <c r="I10" s="14">
+      <c r="K10" s="14">
         <v>12</v>
       </c>
-      <c r="J10" s="6">
+      <c r="L10" s="6">
         <v>0.06</v>
       </c>
-      <c r="K10" s="42">
-        <f>D10+M10+L10-N10-O10-P10</f>
+      <c r="M10" s="41">
+        <f>D10+O10+N10-P10-Q10-R10</f>
         <v>2254454.5916666668</v>
       </c>
-      <c r="L10" s="9">
-        <f>E10*(D10/240)*IF(F10="Diurnas",1.25,IF(F10="Nocturnas",1.75,IF(F10="Festivas",2.5,0)))</f>
+      <c r="N10" s="9">
+        <f t="shared" si="1"/>
         <v>337239.58333333331</v>
       </c>
-      <c r="M10" s="8">
-        <f>IF(D10 &lt;= (Adiccionales!$J$6*2),(G10+Adiccionales!$H$6),G10)</f>
+      <c r="O10" s="8">
+        <f>IF(D10 &lt;= (Adiccionales!$J$6*2),(I10+Adiccionales!$H$6),I10)</f>
         <v>250000</v>
       </c>
-      <c r="N10" s="10">
-        <f t="shared" si="1"/>
+      <c r="P10" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="8">
+      <c r="Q10" s="8">
         <f>(D10*Adiccionales!$F$6) + (D10*Adiccionales!$G$6)</f>
         <v>148000</v>
       </c>
-      <c r="P10" s="10">
-        <f>IF(Q10 &lt;= Adiccionales!$G$11,
+      <c r="R10" s="10">
+        <f>IF(S10 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q10 &lt;= Adiccionales!$H$11,
-       (Q10 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q10 - Adiccionales!$H$11) * 0.02)
+    IF(S10 &lt;= Adiccionales!$H$11,
+       (S10 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S10 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>34784.991666666669</v>
       </c>
-      <c r="Q10" s="8">
-        <f t="shared" si="2"/>
+      <c r="S10" s="8">
+        <f t="shared" si="3"/>
         <v>2237239.5833333335</v>
       </c>
-      <c r="R10" s="10" t="str">
+      <c r="T10" s="10" t="str">
         <f>ROUND(D10/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>37.15 UVT</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-      <c r="C12" s="28"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="46"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1581,60 +1684,62 @@
       <c r="F13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="55"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="10">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="H13" s="8">
+      <c r="J13" s="8">
         <v>20000000</v>
       </c>
-      <c r="I13" s="14">
+      <c r="K13" s="14">
         <v>40</v>
       </c>
-      <c r="J13" s="6">
+      <c r="L13" s="6">
         <v>0.06</v>
       </c>
-      <c r="K13" s="42">
-        <f>D13+M13+L13-N13-O13-P13</f>
+      <c r="M13" s="41">
+        <f>D13+O13+N13-P13-Q13-R13</f>
         <v>57387376.466666669</v>
       </c>
-      <c r="L13" s="9">
-        <f>E13*(D13/240)*IF(F13="Diurnas",1.25,IF(F13="Nocturnas",1.75,IF(F13="Festivas",2.5,0)))</f>
+      <c r="N13" s="9">
+        <f t="shared" si="1"/>
         <v>13020833.333333336</v>
       </c>
-      <c r="M13" s="8">
-        <f>IF(D13 &lt;= (Adiccionales!$J$6*2),(G13+Adiccionales!$H$6),G13)</f>
+      <c r="O13" s="8">
+        <f>IF(D13 &lt;= (Adiccionales!$J$6*2),(I13+Adiccionales!$H$6),I13)</f>
         <v>150000</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="1"/>
+      <c r="P13" s="10">
+        <f t="shared" si="2"/>
         <v>530000</v>
       </c>
-      <c r="O13" s="8">
+      <c r="Q13" s="8">
         <f>(D13*Adiccionales!$F$6) + (D13*Adiccionales!$G$6)</f>
         <v>4000000</v>
       </c>
-      <c r="P13" s="10">
-        <f>IF(Q13 &lt;= Adiccionales!$G$11,
+      <c r="R13" s="10">
+        <f>IF(S13 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q13 &lt;= Adiccionales!$H$11,
-       (Q13 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q13 - Adiccionales!$H$11) * 0.02)
+    IF(S13 &lt;= Adiccionales!$H$11,
+       (S13 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S13 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>1253456.8666666667</v>
       </c>
-      <c r="Q13" s="8">
-        <f t="shared" si="2"/>
+      <c r="S13" s="8">
+        <f t="shared" si="3"/>
         <v>63170833.333333336</v>
       </c>
-      <c r="R13" s="10" t="str">
+      <c r="T13" s="10" t="str">
         <f>ROUND(D13/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>1004.04 UVT</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="57" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1649,60 +1754,62 @@
       <c r="F14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="55"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="10">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="H14" s="8">
+      <c r="J14" s="8">
         <v>0</v>
       </c>
-      <c r="I14" s="14">
+      <c r="K14" s="14">
         <v>0</v>
       </c>
-      <c r="J14" s="6">
+      <c r="L14" s="6">
         <v>0.06</v>
       </c>
-      <c r="K14" s="42">
-        <f>D14+M14+L14-N14-O14-P14</f>
+      <c r="M14" s="41">
+        <f>D14+O14+N14-P14-Q14-R14</f>
         <v>2113302.2999999998</v>
       </c>
-      <c r="L14" s="9">
-        <f>E14*(D14/240)*IF(F14="Diurnas",1.25,IF(F14="Nocturnas",1.75,IF(F14="Festivas",2.5,0)))</f>
+      <c r="N14" s="9">
+        <f t="shared" si="1"/>
         <v>275125</v>
       </c>
-      <c r="M14" s="8">
-        <f>IF(D14 &lt;= (Adiccionales!$J$6*2),(G14+Adiccionales!$H$6),G14)</f>
+      <c r="O14" s="8">
+        <f>IF(D14 &lt;= (Adiccionales!$J$6*2),(I14+Adiccionales!$H$6),I14)</f>
         <v>250000</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="1"/>
+      <c r="P14" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O14" s="8">
+      <c r="Q14" s="8">
         <f>(D14*Adiccionales!$F$6) + (D14*Adiccionales!$G$6)</f>
         <v>140864</v>
       </c>
-      <c r="P14" s="10">
-        <f>IF(Q14 &lt;= Adiccionales!$G$11,
+      <c r="R14" s="10">
+        <f>IF(S14 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q14 &lt;= Adiccionales!$H$11,
-       (Q14 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q14 - Adiccionales!$H$11) * 0.02)
+    IF(S14 &lt;= Adiccionales!$H$11,
+       (S14 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S14 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>31758.7</v>
       </c>
-      <c r="Q14" s="8">
-        <f t="shared" si="2"/>
+      <c r="S14" s="8">
+        <f t="shared" si="3"/>
         <v>2085925</v>
       </c>
-      <c r="R14" s="10" t="str">
+      <c r="T14" s="10" t="str">
         <f>ROUND(D14/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>35.36 UVT</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="57" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1717,60 +1824,62 @@
       <c r="F15" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="55"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="H15" s="8">
+      <c r="J15" s="8">
         <v>2000000</v>
       </c>
-      <c r="I15" s="14">
+      <c r="K15" s="14">
         <v>60</v>
       </c>
-      <c r="J15" s="6">
+      <c r="L15" s="6">
         <v>0.06</v>
       </c>
-      <c r="K15" s="42">
-        <f>D15+M15+L15-N15-O15-P15</f>
+      <c r="M15" s="41">
+        <f>D15+O15+N15-P15-Q15-R15</f>
         <v>2273830.6333333333</v>
       </c>
-      <c r="L15" s="9">
-        <f>E15*(D15/240)*IF(F15="Diurnas",1.25,IF(F15="Nocturnas",1.75,IF(F15="Festivas",2.5,0)))</f>
+      <c r="N15" s="9">
+        <f t="shared" si="1"/>
         <v>150208.33333333334</v>
       </c>
-      <c r="M15" s="8">
-        <f>IF(D15 &lt;= (Adiccionales!$J$6*2),(G15+Adiccionales!$H$6),G15)</f>
+      <c r="O15" s="8">
+        <f>IF(D15 &lt;= (Adiccionales!$J$6*2),(I15+Adiccionales!$H$6),I15)</f>
         <v>300000</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="1"/>
+      <c r="P15" s="10">
+        <f t="shared" si="2"/>
         <v>35333.333333333336</v>
       </c>
-      <c r="O15" s="8">
+      <c r="Q15" s="8">
         <f>(D15*Adiccionales!$F$6) + (D15*Adiccionales!$G$6)</f>
         <v>164800</v>
       </c>
-      <c r="P15" s="10">
-        <f>IF(Q15 &lt;= Adiccionales!$G$11,
+      <c r="R15" s="10">
+        <f>IF(S15 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q15 &lt;= Adiccionales!$H$11,
-       (Q15 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q15 - Adiccionales!$H$11) * 0.02)
+    IF(S15 &lt;= Adiccionales!$H$11,
+       (S15 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S15 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>36244.366666666669</v>
       </c>
-      <c r="Q15" s="8">
-        <f t="shared" si="2"/>
+      <c r="S15" s="8">
+        <f t="shared" si="3"/>
         <v>2310208.3333333335</v>
       </c>
-      <c r="R15" s="10" t="str">
+      <c r="T15" s="10" t="str">
         <f>ROUND(D15/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>41.37 UVT</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="57" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1780,108 +1889,118 @@
         <v>5670500</v>
       </c>
       <c r="E16" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="10">
+        <v>28</v>
+      </c>
+      <c r="G16" s="55">
+        <v>2</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="10">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="H16" s="8">
+      <c r="J16" s="8">
         <v>4000000</v>
       </c>
-      <c r="I16" s="14">
+      <c r="K16" s="14">
         <v>10</v>
       </c>
-      <c r="J16" s="6">
+      <c r="L16" s="6">
         <v>0.06</v>
       </c>
-      <c r="K16" s="42">
-        <f>D16+M16+L16-N16-O16-P16</f>
-        <v>5160573.3833333338</v>
-      </c>
-      <c r="L16" s="9">
-        <f>E16*(D16/240)*IF(F16="Diurnas",1.25,IF(F16="Nocturnas",1.75,IF(F16="Festivas",2.5,0)))</f>
-        <v>330779.16666666663</v>
-      </c>
-      <c r="M16" s="8">
-        <f>IF(D16 &lt;= (Adiccionales!$J$6*2),(G16+Adiccionales!$H$6),G16)</f>
+      <c r="M16" s="41">
+        <f>D16+O16+N16-P16-Q16-R16</f>
+        <v>5096898.3937499998</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" si="1"/>
+        <v>265804.6875</v>
+      </c>
+      <c r="O16" s="8">
+        <f>IF(D16 &lt;= (Adiccionales!$J$6*2),(I16+Adiccionales!$H$6),I16)</f>
         <v>150000</v>
       </c>
-      <c r="N16" s="10">
-        <f t="shared" si="1"/>
+      <c r="P16" s="10">
+        <f t="shared" si="2"/>
         <v>424000</v>
       </c>
-      <c r="O16" s="8">
+      <c r="Q16" s="8">
         <f>(D16*Adiccionales!$F$6) + (D16*Adiccionales!$G$6)</f>
         <v>453640</v>
       </c>
-      <c r="P16" s="10">
-        <f>IF(Q16 &lt;= Adiccionales!$G$11,
+      <c r="R16" s="10">
+        <f>IF(S16 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q16 &lt;= Adiccionales!$H$11,
-       (Q16 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q16 - Adiccionales!$H$11) * 0.02)
+    IF(S16 &lt;= Adiccionales!$H$11,
+       (S16 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S16 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
-        <v>113065.78333333334</v>
-      </c>
-      <c r="Q16" s="8">
-        <f t="shared" si="2"/>
-        <v>6151279.166666667</v>
-      </c>
-      <c r="R16" s="10" t="str">
+        <v>111766.29375000001</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" si="3"/>
+        <v>6086304.6875</v>
+      </c>
+      <c r="T16" s="10" t="str">
         <f>ROUND(D16/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>113.87 UVT</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="24"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="27"/>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="48"/>
-      <c r="C18" s="28"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="24"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="27"/>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="2:19" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+    </row>
+    <row r="19" spans="2:21" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="42" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="25">
@@ -1893,63 +2012,65 @@
       <c r="F19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="56"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="10">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="H19" s="11">
+      <c r="J19" s="11">
         <v>300000</v>
       </c>
-      <c r="I19" s="18">
+      <c r="K19" s="18">
         <v>15</v>
       </c>
-      <c r="J19" s="27">
+      <c r="L19" s="26">
         <v>0.06</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="M19" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="26">
-        <f>E19*(D19/240)*IF(F19="Diurnas",1.25,IF(F19="Nocturnas",1.75,IF(F19="Festivas",2.5,0)))</f>
+      <c r="N19" s="9">
+        <f t="shared" si="1"/>
         <v>-109375.00000000001</v>
       </c>
-      <c r="M19" s="8">
-        <f>IF(D19 &lt;= (Adiccionales!$J$6*2),(G19+Adiccionales!$H$6),G19)</f>
+      <c r="O19" s="8">
+        <f>IF(D19 &lt;= (Adiccionales!$J$6*2),(I19+Adiccionales!$H$6),I19)</f>
         <v>250000</v>
       </c>
-      <c r="N19" s="10">
-        <f t="shared" si="1"/>
+      <c r="P19" s="10">
+        <f t="shared" si="2"/>
         <v>21200</v>
       </c>
-      <c r="O19" s="8">
+      <c r="Q19" s="8">
         <f>(D19*Adiccionales!$F$6) + (D19*Adiccionales!$G$6)</f>
         <v>-80000</v>
       </c>
-      <c r="P19" s="10">
-        <f>IF(Q19 &lt;= Adiccionales!$G$11,
+      <c r="R19" s="10">
+        <f>IF(S19 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q19 &lt;= Adiccionales!$H$11,
-       (Q19 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q19 - Adiccionales!$H$11) * 0.02)
+    IF(S19 &lt;= Adiccionales!$H$11,
+       (S19 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S19 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="8">
-        <f t="shared" si="2"/>
+      <c r="S19" s="8">
+        <f t="shared" si="3"/>
         <v>-1059375</v>
       </c>
-      <c r="R19" s="15" t="str">
+      <c r="T19" s="15" t="str">
         <f>ROUND(D19/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>-20.08 UVT</v>
       </c>
-      <c r="S19" s="35"/>
-    </row>
-    <row r="20" spans="2:19" ht="54" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="U19" s="34"/>
+    </row>
+    <row r="20" spans="2:21" ht="54" x14ac:dyDescent="0.25">
+      <c r="B20" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="42" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="11">
@@ -1961,249 +2082,275 @@
       <c r="F20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="56"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="10">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="H20" s="11">
+      <c r="J20" s="11">
         <v>600000</v>
       </c>
-      <c r="I20" s="18">
+      <c r="K20" s="18">
         <v>32</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19" t="s">
+      <c r="L20" s="18"/>
+      <c r="M20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="19" t="s">
+      <c r="N20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="8">
-        <f>IF(D20 &lt;= (Adiccionales!$J$6*2),(G20+Adiccionales!$H$6),G20)</f>
+      <c r="O20" s="8">
+        <f>IF(D20 &lt;= (Adiccionales!$J$6*2),(I20+Adiccionales!$H$6),I20)</f>
         <v>250000</v>
       </c>
-      <c r="N20" s="10">
-        <f t="shared" si="1"/>
+      <c r="P20" s="10">
+        <f t="shared" si="2"/>
         <v>18750</v>
       </c>
-      <c r="O20" s="8">
+      <c r="Q20" s="8">
         <f>(D20*Adiccionales!$F$6) + (D20*Adiccionales!$G$6)</f>
         <v>132016</v>
       </c>
-      <c r="P20" s="10" t="e">
-        <f>IF(Q20 &lt;= Adiccionales!$G$11,
+      <c r="R20" s="10" t="e">
+        <f>IF(S20 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q20 &lt;= Adiccionales!$H$11,
-       (Q20 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q20 - Adiccionales!$H$11) * 0.02)
+    IF(S20 &lt;= Adiccionales!$H$11,
+       (S20 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S20 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q20" s="8" t="e">
-        <f t="shared" si="2"/>
+      <c r="S20" s="8" t="e">
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R20" s="15" t="str">
+      <c r="T20" s="15" t="str">
         <f>ROUND(D20/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>33.14 UVT</v>
       </c>
-      <c r="S20" s="35"/>
-    </row>
-    <row r="21" spans="2:19" ht="27" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="U20" s="34"/>
+    </row>
+    <row r="21" spans="2:21" ht="27" x14ac:dyDescent="0.25">
+      <c r="B21" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="42" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="11">
         <v>1560300</v>
       </c>
-      <c r="E21" s="44">
+      <c r="E21" s="43">
         <v>-10</v>
       </c>
       <c r="F21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="56"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="10">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="H21" s="11">
+      <c r="J21" s="11">
         <v>0</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="45">
+      <c r="K21" s="18"/>
+      <c r="L21" s="44">
         <v>0.06</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="M21" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="26">
-        <f>E21*(D21/240)*IF(F21="Diurnas",1.25,IF(F21="Nocturnas",1.75,IF(F21="Festivas",2.5,0)))</f>
+      <c r="N21" s="9">
+        <f t="shared" si="1"/>
         <v>-81265.625</v>
       </c>
-      <c r="M21" s="8">
-        <f>IF(D21 &lt;= (Adiccionales!$J$6*2),(G21+Adiccionales!$H$6),G21)</f>
+      <c r="O21" s="8">
+        <f>IF(D21 &lt;= (Adiccionales!$J$6*2),(I21+Adiccionales!$H$6),I21)</f>
         <v>300000</v>
       </c>
-      <c r="N21" s="10">
-        <f t="shared" si="1"/>
+      <c r="P21" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="8">
+      <c r="Q21" s="8">
         <f>(D21*Adiccionales!$F$6) + (D21*Adiccionales!$G$6)</f>
         <v>124824</v>
       </c>
-      <c r="P21" s="10">
-        <f>IF(Q21 &lt;= Adiccionales!$G$11,
+      <c r="R21" s="10">
+        <f>IF(S21 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q21 &lt;= Adiccionales!$H$11,
-       (Q21 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q21 - Adiccionales!$H$11) * 0.02)
+    IF(S21 &lt;= Adiccionales!$H$11,
+       (S21 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S21 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
         <v>21620.887500000001</v>
       </c>
-      <c r="Q21" s="8">
-        <f t="shared" si="2"/>
+      <c r="S21" s="8">
+        <f t="shared" si="3"/>
         <v>1579034.375</v>
       </c>
-      <c r="R21" s="15" t="str">
+      <c r="T21" s="15" t="str">
         <f>ROUND(D21/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>31.33 UVT</v>
       </c>
-      <c r="S21" s="35"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="U21" s="34"/>
+    </row>
+    <row r="22" spans="2:21" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="42" t="s">
         <v>48</v>
       </c>
       <c r="D22" s="11">
         <v>4350000</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="10">
+      <c r="E22" s="43">
+        <v>16</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="20">
+        <v>16</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="10">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="H22" s="11">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="46">
-        <f>D22+G22+L22-N22</f>
-        <v>4500000</v>
-      </c>
-      <c r="L22" s="26">
-        <f>E22*(D22/240)*IF(F22="Diurnas",1.25,IF(F22="Nocturnas",1.75,IF(F22="Festivas",2.5,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="8">
-        <f>IF(D22 &lt;= (Adiccionales!$J$6*2),(G22+Adiccionales!$H$6),G22)</f>
+      <c r="J22" s="11">
+        <v>500000</v>
+      </c>
+      <c r="K22" s="16">
+        <v>10</v>
+      </c>
+      <c r="L22" s="59">
+        <v>0.06</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="9">
+        <f t="shared" si="1"/>
+        <v>870000</v>
+      </c>
+      <c r="O22" s="8">
+        <f>IF(D22 &lt;= (Adiccionales!$J$6*2),(I22+Adiccionales!$H$6),I22)</f>
         <v>150000</v>
       </c>
-      <c r="N22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="8">
+      <c r="P22" s="10">
+        <f t="shared" si="2"/>
+        <v>53000</v>
+      </c>
+      <c r="Q22" s="8">
         <f>(D22*Adiccionales!$F$6) + (D22*Adiccionales!$G$6)</f>
         <v>348000</v>
       </c>
-      <c r="P22" s="10">
-        <f>IF(Q22 &lt;= Adiccionales!$G$11,
+      <c r="R22" s="10">
+        <f>IF(S22 &lt;= Adiccionales!$G$11,
     0,
-    IF(Q22 &lt;= Adiccionales!$H$11,
-       (Q22 - Adiccionales!$G$11) * 0.01,
-       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((Q22 - Adiccionales!$H$11) * 0.02)
+    IF(S22 &lt;= Adiccionales!$H$11,
+       (S22 - Adiccionales!$G$11) * 0.01,
+       ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S22 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
-        <v>80040.200000000012</v>
-      </c>
-      <c r="Q22" s="8">
-        <f t="shared" si="2"/>
-        <v>4500000</v>
-      </c>
-      <c r="R22" s="15" t="str">
+        <v>97440.200000000012</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="3"/>
+        <v>5370000</v>
+      </c>
+      <c r="T22" s="15" t="str">
         <f>ROUND(D22/Adiccionales!$I$6,2) &amp; " UVT"</f>
         <v>87.35 UVT</v>
       </c>
-      <c r="S22" s="35"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
+      <c r="U22" s="34"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="40"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
-      <c r="S23" s="35"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="35"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="34"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="34"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="L26" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="K4:R5"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="M4:T5"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2214,7 +2361,7 @@
           <x14:formula1>
             <xm:f>Adiccionales!$C$5:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F21:F22 F19 F13:F16 F7:F10</xm:sqref>
+          <xm:sqref>H19 H13:H16 H7:H10 F7:F10 F13:F16 F19 F21:F22 H21:H22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4517697C-3FF4-49BB-BEB3-8BC087888680}">
           <x14:formula1>
@@ -2245,108 +2392,108 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="55"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="32" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="32" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="30">
+      <c r="E6" s="30"/>
+      <c r="F6" s="29">
         <v>0.04</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>0.04</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <v>200000</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="28">
         <v>49799</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="28">
         <v>1423500</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="37">
         <v>50000</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <f>4*I6</f>
         <v>199196</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="37">
         <f>16*I6</f>
         <v>796784</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="37">
         <v>100000</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="37">
         <v>150000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correción caso de error 4
</commit_message>
<xml_diff>
--- a/Liquidador-de-Nómina.xlsx
+++ b/Liquidador-de-Nómina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/A0A66C4E88FB0D17/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b12s307\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{FDE5CBCE-8AF8-41F9-BF5D-FC43121CB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B35B6DDB-FF38-4818-AFFB-1634E97145A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C36A8BD-90AF-4354-A5EF-AAEDDF3CCF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC24777-1EF7-4777-BC9E-05463E1B662D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="23730" windowHeight="10530" xr2:uid="{ACC24777-1EF7-4777-BC9E-05463E1B662D}"/>
   </bookViews>
   <sheets>
     <sheet name="Nómina" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luis Guerra:</t>
         </r>
@@ -209,7 +209,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Si el trabajor tiene horas extras en diferentes turnos estas se suman y se aplica el factor correspondiente</t>
@@ -224,7 +224,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luis Guerra:</t>
         </r>
@@ -236,7 +236,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-El limite al mes es de 30 horas y el empleado tiene 32</t>
+El limite al mes es de 50 horas y el empleado tiene 51</t>
         </r>
       </text>
     </comment>
@@ -252,10 +252,19 @@
   <commentList>
     <comment ref="J5" authorId="0" shapeId="0" xr:uid="{8CEB451D-CE14-469B-ACD3-0E2DAA3469EB}">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Salario mínimo legal vigente en 2025</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -444,10 +453,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;XDR&quot;* #,##0.00_-;\-&quot;XDR&quot;* #,##0.00_-;_-&quot;XDR&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;XDR&quot;* #,##0.00_-;\-&quot;XDR&quot;* #,##0.00_-;_-&quot;XDR&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,17 +508,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="19">
@@ -685,9 +689,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -710,16 +714,16 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -731,7 +735,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,13 +747,13 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -758,10 +762,10 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -799,7 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -814,6 +818,23 @@
     <xf numFmtId="9" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -841,22 +862,6 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1214,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10311B7A-29B6-449E-A833-BFA5BF788BF0}">
   <dimension ref="B4:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,53 +1244,53 @@
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="48" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51" t="s">
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
     </row>
     <row r="6" spans="2:20" ht="27" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -1347,7 +1352,7 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1362,7 +1367,7 @@
       <c r="F7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="13"/>
       <c r="I7" s="10">
         <f>IF(C7="Empleado nuevo",50000,IF(C7="Empleado antiguo",100000,IF(C7="Administrador",150000,0)))</f>
@@ -1417,7 +1422,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1430,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="55"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="13"/>
       <c r="I8" s="10">
         <f t="shared" ref="I8:I22" si="0">IF(C8="Empleado nuevo",50000,IF(C8="Empleado antiguo",100000,IF(C8="Administrador",150000,0)))</f>
@@ -1485,7 +1490,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1500,7 +1505,7 @@
       <c r="F9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="55"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="13"/>
       <c r="I9" s="10">
         <f t="shared" si="0"/>
@@ -1555,7 +1560,7 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="48" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1570,7 +1575,7 @@
       <c r="F10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="55"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="13"/>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
@@ -1625,7 +1630,7 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="53" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="27"/>
@@ -1648,7 +1653,7 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="27"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
@@ -1669,7 +1674,7 @@
       <c r="T12" s="24"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="48" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1684,7 +1689,7 @@
       <c r="F13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="13"/>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
@@ -1739,7 +1744,7 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="48" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1754,7 +1759,7 @@
       <c r="F14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="13"/>
       <c r="I14" s="10">
         <f t="shared" si="0"/>
@@ -1809,7 +1814,7 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="48" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1824,7 +1829,7 @@
       <c r="F15" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="55"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="13"/>
       <c r="I15" s="10">
         <f t="shared" si="0"/>
@@ -1879,7 +1884,7 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="48" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1894,7 +1899,7 @@
       <c r="F16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16" s="46">
         <v>2</v>
       </c>
       <c r="H16" s="13" t="s">
@@ -1953,7 +1958,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="27"/>
@@ -1976,7 +1981,7 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="27"/>
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
@@ -1997,7 +2002,7 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:21" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="42" t="s">
@@ -2012,7 +2017,7 @@
       <c r="F19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="56"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="17"/>
       <c r="I19" s="10">
         <f t="shared" si="0"/>
@@ -2067,7 +2072,7 @@
       <c r="U19" s="34"/>
     </row>
     <row r="20" spans="2:21" ht="54" x14ac:dyDescent="0.25">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="42" t="s">
@@ -2082,7 +2087,7 @@
       <c r="F20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="56"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="17"/>
       <c r="I20" s="10">
         <f t="shared" si="0"/>
@@ -2134,7 +2139,7 @@
       <c r="U20" s="34"/>
     </row>
     <row r="21" spans="2:21" ht="27" x14ac:dyDescent="0.25">
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="42" t="s">
@@ -2149,7 +2154,7 @@
       <c r="F21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="56"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="17"/>
       <c r="I21" s="10">
         <f t="shared" si="0"/>
@@ -2202,7 +2207,7 @@
       <c r="U21" s="34"/>
     </row>
     <row r="22" spans="2:21" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="42" t="s">
@@ -2212,13 +2217,13 @@
         <v>4350000</v>
       </c>
       <c r="E22" s="43">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>29</v>
       </c>
       <c r="G22" s="20">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>28</v>
@@ -2233,7 +2238,7 @@
       <c r="K22" s="16">
         <v>10</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L22" s="50">
         <v>0.06</v>
       </c>
       <c r="M22" s="19" t="s">
@@ -2241,7 +2246,7 @@
       </c>
       <c r="N22" s="9">
         <f t="shared" si="1"/>
-        <v>870000</v>
+        <v>1391093.75</v>
       </c>
       <c r="O22" s="8">
         <f>IF(D22 &lt;= (Adiccionales!$J$6*2),(I22+Adiccionales!$H$6),I22)</f>
@@ -2263,11 +2268,11 @@
        ((Adiccionales!$H$11 - Adiccionales!$G$11) * 0.01) + ((S22 - Adiccionales!$H$11) * 0.02)
       )
    )</f>
-        <v>97440.200000000012</v>
+        <v>107862.07500000001</v>
       </c>
       <c r="S22" s="8">
         <f t="shared" si="3"/>
-        <v>5370000</v>
+        <v>5891093.75</v>
       </c>
       <c r="T22" s="15" t="str">
         <f>ROUND(D22/Adiccionales!$I$6,2) &amp; " UVT"</f>
@@ -2341,7 +2346,8 @@
       <c r="U25" s="34"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="L26" s="60"/>
+      <c r="L26" s="51"/>
+      <c r="O26" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2395,14 +2401,14 @@
       <c r="C4" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="28" t="s">

</xml_diff>